<commit_message>
UP TO DATE 14/06
</commit_message>
<xml_diff>
--- a/Foot_Mapa_excell.xlsx
+++ b/Foot_Mapa_excell.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="40" yWindow="460" windowWidth="28160" windowHeight="15620" tabRatio="500"/>
+    <workbookView xWindow="7080" yWindow="460" windowWidth="28160" windowHeight="15620" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -29,9 +29,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="31">
   <si>
-    <t>FISHING.GUILD</t>
-  </si>
-  <si>
     <t>SOCIOECOLOGICAL_VUL</t>
   </si>
   <si>
@@ -120,6 +117,9 @@
   </si>
   <si>
     <t>Porto de Som</t>
+  </si>
+  <si>
+    <t>fishing.guild</t>
   </si>
 </sst>
 </file>
@@ -436,208 +436,206 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C18"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="G16" sqref="G16"/>
-    </sheetView>
+    <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
+        <v>30</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
       <c r="C1" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B2">
-        <v>0.318</v>
+        <v>0.64351199921351798</v>
       </c>
       <c r="C2" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B3">
-        <v>0.88700000000000001</v>
+        <v>1.44803055592082</v>
       </c>
       <c r="C3" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B4">
-        <v>0.24399999999999999</v>
+        <v>0.47973585662181201</v>
       </c>
       <c r="C4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B5">
-        <v>0.67600000000000005</v>
+        <v>1.3506439739467599</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B6">
-        <v>0.57399999999999995</v>
+        <v>1.0055151004343701</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B7">
-        <v>0.61799999999999999</v>
+        <v>1.20973199935969</v>
       </c>
       <c r="C7" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B8">
-        <v>0.17699999999999999</v>
+        <v>0.76697890506139099</v>
       </c>
       <c r="C8" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B9">
-        <v>0.56399999999999995</v>
+        <v>1.20414078778463</v>
       </c>
       <c r="C9" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="B10">
-        <v>0.20399999999999999</v>
+        <v>0.92651538155755897</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="B11">
-        <v>0.98899999999999999</v>
+        <v>1.4164291610642299</v>
       </c>
       <c r="C11" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B12">
-        <v>0.06</v>
+        <v>0.98288821706572604</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B13">
-        <v>-0.08</v>
+        <v>0.69910834085535301</v>
       </c>
       <c r="C13" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B14">
-        <v>1.0329999999999999</v>
+        <v>1.4772391685533599</v>
       </c>
       <c r="C14" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15">
-        <v>-9.5000000000000001E-2</v>
+        <v>0.89540092932601401</v>
       </c>
       <c r="C15" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B16">
-        <v>0.53200000000000003</v>
+        <v>1.2381599474816201</v>
       </c>
       <c r="C16" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="17" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B17">
-        <v>0.58899999999999997</v>
+        <v>1.15956085361765</v>
       </c>
       <c r="C17" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
     </row>
     <row r="18" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B18">
-        <v>0.45100000000000001</v>
+        <v>1.07955789983748</v>
       </c>
       <c r="C18" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
     </row>
   </sheetData>

</xml_diff>